<commit_message>
Quiz mit neuem Datensatz
</commit_message>
<xml_diff>
--- a/Module/Fragen_Quiz.xlsx
+++ b/Module/Fragen_Quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Documents\R-Projekte\HackathonSN2023\Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA7F49F-E4A7-4CB8-B531-FB108CB643A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1BC759-BC09-4ABC-AFB5-386983C8983D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{038BF83B-4E0E-466C-A2A8-7B82ACCE286C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>Frage</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Land- und Forstwirtschaft, Fischerei (A)</t>
+  </si>
+  <si>
+    <t>Wert_Code</t>
+  </si>
+  <si>
+    <t>BEVSTD__Bevoelkerungsstand__Anzahl</t>
+  </si>
+  <si>
+    <t>ID0002__Erwerbstaetige_im_Jahresdurchschnitt__1000</t>
   </si>
 </sst>
 </file>
@@ -554,9 +563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6939AAD5-29F7-409B-8D31-2C6001871F5E}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -569,7 +580,7 @@
     <col min="9" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -600,8 +611,11 @@
       <c r="J1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12411</v>
       </c>
@@ -630,8 +644,11 @@
       <c r="J2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13312</v>
       </c>
@@ -659,6 +676,9 @@
       </c>
       <c r="J3" t="s">
         <v>51</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Anpassung Fragen und Quiz
</commit_message>
<xml_diff>
--- a/Module/Fragen_Quiz.xlsx
+++ b/Module/Fragen_Quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Documents\R-Projekte\HackathonSN2023\Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4456B8F-3B49-4958-AD8D-C536C3D30E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13129A09-144E-4E09-B8A0-31C3C7EFB5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{038BF83B-4E0E-466C-A2A8-7B82ACCE286C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Fragen" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fragen!$A$1:$H$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fragen!$A$1:$H$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>Frage</t>
   </si>
@@ -131,9 +131,6 @@
     <t>In welcher Stadt oder welchem Landkreis wurden die meisten Baugenehmigungen für Wohngebäude erteilt?</t>
   </si>
   <si>
-    <t>In welcher Stadt oder welchem Landkreis wird am meisten der Bodenfläche für Landwirtschaft genutzt?</t>
-  </si>
-  <si>
     <t>In welcher Stadt oder welchem Landkreis hat die meiste Waldfläche?</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>min</t>
   </si>
   <si>
-    <t>BEV519__Durchschnittsalter_der_Bevoelkerung__Jahre…</t>
-  </si>
-  <si>
     <t>ID0002__Erwerbstaetige_im_Jahresdurchschnitt__1000</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>FLC005__Bodenflaeche__ha</t>
   </si>
   <si>
-    <t>Landwirtschaft</t>
-  </si>
-  <si>
     <t>Wald</t>
   </si>
   <si>
@@ -252,6 +243,12 @@
   </si>
   <si>
     <t>EKM014__verfueg._Einkommen_der_priv._Haushalte_je_Einwohner__EUR</t>
+  </si>
+  <si>
+    <t>insgesamt</t>
+  </si>
+  <si>
+    <t>BEV519__Durchschnittsalter_der_Bevoelkerung__Jahre...</t>
   </si>
 </sst>
 </file>
@@ -603,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75852A4-ECA2-454E-AC82-6219A7C78EC0}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,19 +622,19 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -651,19 +648,19 @@
         <v>11111</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
         <v>22</v>
@@ -677,19 +674,19 @@
         <v>12411</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>23</v>
@@ -703,19 +700,19 @@
         <v>12411</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -729,19 +726,19 @@
         <v>13312</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -755,19 +752,19 @@
         <v>21111</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
@@ -781,19 +778,19 @@
         <v>21111</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
@@ -807,19 +804,19 @@
         <v>21311</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
         <v>28</v>
@@ -833,19 +830,19 @@
         <v>31111</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -859,19 +856,19 @@
         <v>33111</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
         <v>30</v>
@@ -882,54 +879,54 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>33111</v>
+        <v>41241</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>41241</v>
+        <v>45412</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,159 +934,133 @@
         <v>45412</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>45412</v>
+        <v>46251</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
         <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>46251</v>
+        <v>53111</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
         <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>53111</v>
+        <v>61511</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
         <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>61511</v>
+        <v>82411</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
         <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>82411</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H18" xr:uid="{C75852A4-ECA2-454E-AC82-6219A7C78EC0}"/>
+  <autoFilter ref="A1:H17" xr:uid="{C75852A4-ECA2-454E-AC82-6219A7C78EC0}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix App 3 plots
</commit_message>
<xml_diff>
--- a/Module/Fragen_Quiz.xlsx
+++ b/Module/Fragen_Quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Documents\R-Projekte\HackathonSN2023\Module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DBC932-D461-4163-A0BE-1F68AA4EA338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC1C3B3-2CC1-43F9-8977-06890A164B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{038BF83B-4E0E-466C-A2A8-7B82ACCE286C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>Frage</t>
   </si>
@@ -116,9 +116,6 @@
     <t>In welcher Stadt oder welchem Landkreis wurden die meisten Baugenehmigungen für Wohngebäude erteilt?</t>
   </si>
   <si>
-    <t>In welcher Stadt oder welchem Landkreis hat die meiste Waldfläche?</t>
-  </si>
-  <si>
     <t>In welcher Stadt oder welchem Landkreis werden die meisten Kartoffeln pro Hektar geerntet?</t>
   </si>
   <si>
@@ -252,6 +249,12 @@
   </si>
   <si>
     <t>Die VGR (Volkswirtschaftliche Gesamtrechnung) der Länder berechnet u.a. das verfügbare Einkommen der privaten Haushalte je Einwohner.</t>
+  </si>
+  <si>
+    <t>Welche Stadt oder welcher Landkreis hat die meiste Waldfläche?</t>
+  </si>
+  <si>
+    <t>Personenkraftwagen</t>
   </si>
 </sst>
 </file>
@@ -606,7 +609,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,19 +628,19 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -651,19 +654,19 @@
         <v>11111</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -677,19 +680,19 @@
         <v>12411</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>18</v>
@@ -703,25 +706,25 @@
         <v>12411</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,19 +732,19 @@
         <v>13312</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -755,19 +758,19 @@
         <v>21111</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -781,19 +784,19 @@
         <v>21111</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -807,19 +810,19 @@
         <v>21311</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
@@ -833,19 +836,19 @@
         <v>31111</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -859,22 +862,22 @@
         <v>33111</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s">
         <v>9</v>
@@ -885,25 +888,25 @@
         <v>41241</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -911,25 +914,25 @@
         <v>45412</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,22 +940,22 @@
         <v>45412</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" t="s">
         <v>10</v>
@@ -963,22 +966,22 @@
         <v>46251</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
@@ -989,25 +992,25 @@
         <v>53111</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,22 +1018,22 @@
         <v>61511</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -1041,25 +1044,25 @@
         <v>82411</v>
       </c>
       <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" t="s">
-        <v>65</v>
-      </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>